<commit_message>
Replace RPEpUACE with Brazil specific data
</commit_message>
<xml_diff>
--- a/InputData/land/RPEpUACE/Rebound Pol Emis per Unit Avoided CO2 Emis.xlsx
+++ b/InputData/land/RPEpUACE/Rebound Pol Emis per Unit Avoided CO2 Emis.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\land\RPEpUACE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ssy02/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0C39C8-7140-4E9A-800C-6D86145E4794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E178A6-553F-6D4A-848F-2955EE338B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="21380" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="2" r:id="rId2"/>
-    <sheet name="RPEpUACE" sheetId="3" r:id="rId3"/>
+    <sheet name="Data_US" sheetId="2" r:id="rId2"/>
+    <sheet name="Data_Brazil" sheetId="4" r:id="rId3"/>
+    <sheet name="RPEpUACE" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="71">
   <si>
     <t>RPEpUACE Rebound Pollutant Emissions per Unit Avoided CO2 Emissions</t>
   </si>
@@ -42,9 +44,6 @@
     <t>Source:</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>For each (net) gram of CO2 abated via LULUCF, there is a positive amount of CH4</t>
   </si>
   <si>
@@ -217,6 +216,39 @@
   </si>
   <si>
     <t>N2O/CO2 Ratio</t>
+  </si>
+  <si>
+    <t>Brazil SEEG</t>
+  </si>
+  <si>
+    <t>Overall Table of national and state data</t>
+  </si>
+  <si>
+    <t>Base de Dados de Emissões e Remoções de Gases de Efeito Estufa no Brasil (1970-2023): Estados e biomas</t>
+  </si>
+  <si>
+    <t>Consulta Série Histórica Table</t>
+  </si>
+  <si>
+    <t>https://seeg.eco.br/en/seeg-data/</t>
+  </si>
+  <si>
+    <t>US-Notes</t>
+  </si>
+  <si>
+    <t>Brazil-Notes</t>
+  </si>
+  <si>
+    <t>Emissions (t)</t>
+  </si>
+  <si>
+    <t>Removal (t)</t>
+  </si>
+  <si>
+    <t>Net (t)</t>
+  </si>
+  <si>
+    <t>X/CO2 Ratio (dimensionless)</t>
   </si>
 </sst>
 </file>
@@ -269,7 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -278,6 +310,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -297,9 +332,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -337,9 +372,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -372,26 +407,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -424,26 +442,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -617,75 +618,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" s="4">
         <v>2022</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>7</v>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -698,34 +734,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>25</v>
       </c>
       <c r="B4">
         <v>2016</v>
@@ -743,9 +779,9 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="5">
         <v>-862045</v>
@@ -763,9 +799,9 @@
         <v>-812176</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="5">
         <v>-725571</v>
@@ -783,9 +819,9 @@
         <v>-668057</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="5">
         <v>-99454</v>
@@ -803,9 +839,9 @@
         <v>-99521</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="5">
         <v>-22731</v>
@@ -823,9 +859,9 @@
         <v>-23335</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="5">
         <v>54107</v>
@@ -843,9 +879,9 @@
         <v>54380</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="5">
         <v>7958</v>
@@ -863,9 +899,9 @@
         <v>4497</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="5">
         <v>-22553</v>
@@ -883,9 +919,9 @@
         <v>-24101</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="5">
         <v>-8046</v>
@@ -903,9 +939,9 @@
         <v>-8084</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13">
         <v>254</v>
@@ -923,9 +959,9 @@
         <v>279</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="5">
         <v>-123794</v>
@@ -943,9 +979,9 @@
         <v>-126128</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="5">
         <v>77784</v>
@@ -963,9 +999,9 @@
         <v>77895</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="5">
         <v>1131</v>
@@ -983,9 +1019,9 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17">
         <v>154</v>
@@ -1003,9 +1039,9 @@
         <v>545</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1023,9 +1059,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19">
         <v>11</v>
@@ -1043,9 +1079,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20">
         <v>796.7</v>
@@ -1063,9 +1099,9 @@
         <v>797</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21">
         <v>153</v>
@@ -1083,29 +1119,29 @@
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
         <v>42</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>43</v>
-      </c>
-      <c r="C22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>44</v>
       </c>
       <c r="B23">
         <v>7</v>
@@ -1123,9 +1159,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24">
         <v>8</v>
@@ -1143,9 +1179,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -1163,9 +1199,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26">
         <v>13</v>
@@ -1183,9 +1219,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -1203,29 +1239,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>38</v>
-      </c>
-      <c r="B28" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" t="s">
-        <v>43</v>
-      </c>
-      <c r="F28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>39</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1243,15 +1279,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1263,29 +1299,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" t="s">
         <v>42</v>
       </c>
-      <c r="B31" t="s">
-        <v>43</v>
-      </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F31" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -1303,49 +1339,49 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B43" s="3">
         <f>B16/B5</f>
@@ -1368,9 +1404,9 @@
         <v>-1.8739780540178485E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B44" s="3">
         <f>B25/B5</f>
@@ -1399,119 +1435,485 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{033752E3-E281-4A89-AA6F-E6EEA52BB3CF}">
+  <dimension ref="A1:U14"/>
+  <sheetViews>
+    <sheetView zoomScale="91" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:U14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>2016</v>
+      </c>
+      <c r="C2">
+        <v>2017</v>
+      </c>
+      <c r="D2">
+        <v>2018</v>
+      </c>
+      <c r="E2">
+        <v>2019</v>
+      </c>
+      <c r="F2">
+        <v>2020</v>
+      </c>
+      <c r="G2">
+        <v>2016</v>
+      </c>
+      <c r="H2">
+        <v>2017</v>
+      </c>
+      <c r="I2">
+        <v>2018</v>
+      </c>
+      <c r="J2">
+        <v>2019</v>
+      </c>
+      <c r="K2">
+        <v>2020</v>
+      </c>
+      <c r="L2">
+        <v>2016</v>
+      </c>
+      <c r="M2">
+        <v>2017</v>
+      </c>
+      <c r="N2">
+        <v>2018</v>
+      </c>
+      <c r="O2">
+        <v>2019</v>
+      </c>
+      <c r="P2">
+        <v>2020</v>
+      </c>
+      <c r="Q2">
+        <v>2016</v>
+      </c>
+      <c r="R2">
+        <v>2017</v>
+      </c>
+      <c r="S2">
+        <v>2018</v>
+      </c>
+      <c r="T2">
+        <v>2019</v>
+      </c>
+      <c r="U2">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>912451471.0575484</v>
+      </c>
+      <c r="C3">
+        <v>799395887.88613808</v>
+      </c>
+      <c r="D3">
+        <v>840903929.12567472</v>
+      </c>
+      <c r="E3">
+        <v>1132761396.5100524</v>
+      </c>
+      <c r="F3">
+        <v>1051399361.4150835</v>
+      </c>
+      <c r="G3">
+        <v>-623687858.70208669</v>
+      </c>
+      <c r="H3">
+        <v>-628247802.8205142</v>
+      </c>
+      <c r="I3">
+        <v>-638693631.25603342</v>
+      </c>
+      <c r="J3">
+        <v>-644491082.17767024</v>
+      </c>
+      <c r="K3">
+        <v>-650113306.53333974</v>
+      </c>
+      <c r="L3">
+        <f>SUM(B3,G3)</f>
+        <v>288763612.35546172</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:P3" si="0">SUM(C3,H3)</f>
+        <v>171148085.06562388</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>202210297.8696413</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="0"/>
+        <v>488270314.3323822</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="0"/>
+        <v>401286054.88174379</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>1171104.8360813039</v>
+      </c>
+      <c r="C12">
+        <v>1011163.4367387437</v>
+      </c>
+      <c r="D12">
+        <v>1075773.9708492672</v>
+      </c>
+      <c r="E12">
+        <v>1491899.7001309432</v>
+      </c>
+      <c r="F12">
+        <v>1395987.8551887732</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f>SUM(B12,G12)</f>
+        <v>1171104.8360813039</v>
+      </c>
+      <c r="M12">
+        <f t="shared" ref="M12:P13" si="1">SUM(C12,H12)</f>
+        <v>1011163.4367387437</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>1075773.9708492672</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="1"/>
+        <v>1491899.7001309432</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="1"/>
+        <v>1395987.8551887732</v>
+      </c>
+      <c r="Q12">
+        <f>L12/L$3</f>
+        <v>4.0555831343448475E-3</v>
+      </c>
+      <c r="R12">
+        <f t="shared" ref="R12:U13" si="2">M12/M$3</f>
+        <v>5.9081200724567257E-3</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="2"/>
+        <v>5.3200751009366753E-3</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="2"/>
+        <v>3.0554790171318019E-3</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="2"/>
+        <v>3.4787848673190529E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>35812.832140328195</v>
+      </c>
+      <c r="C13">
+        <v>31006.487909109856</v>
+      </c>
+      <c r="D13">
+        <v>32930.025050654251</v>
+      </c>
+      <c r="E13">
+        <v>45664.090178815</v>
+      </c>
+      <c r="F13">
+        <v>42583.341777824389</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ref="L13" si="3">SUM(B13,G13)</f>
+        <v>35812.832140328195</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>31006.487909109856</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>32930.025050654251</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="1"/>
+        <v>45664.090178815</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="1"/>
+        <v>42583.341777824389</v>
+      </c>
+      <c r="Q13">
+        <f>L13/L$3</f>
+        <v>1.2402127764021522E-4</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="2"/>
+        <v>1.8116760054441119E-4</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="2"/>
+        <v>1.6285038594761981E-4</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="2"/>
+        <v>9.3522151231438373E-5</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="2"/>
+        <v>1.0611717317307077E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="Q1:U1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.36328125" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="B11" s="3">
+        <f>AVERAGE(Data_Brazil!Q12:U12)</f>
+        <v>4.3636084384378205E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3">
+        <f>AVERAGE(Data_Brazil!Q13:U13)</f>
+        <v>1.335357177073511E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>19</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3">
-        <f>-AVERAGE(Data!B43:F43)</f>
-        <v>1.5377230909479366E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3">
-        <f>-AVERAGE(Data!B44:F44)</f>
-        <v>3.9432013528689668E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>20</v>
       </c>
       <c r="B13">
         <v>0</v>

</xml_diff>